<commit_message>
Initial commit for Render deployment
</commit_message>
<xml_diff>
--- a/forensic_cases.xlsx
+++ b/forensic_cases.xlsx
@@ -12,6 +12,7 @@
     <sheet name="cases" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="samples" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="custody_events" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="lab_results" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,6 +469,42 @@
           <t>api_token</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>created_at</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>admin@fasttrack.local</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$2jDA8TMQ61QO1h39$05fa170edb747deedcfd99b0a23d8c004425219406ccb6a0309c5b9dc6df63ac0b5ac98dd4d238fed4523aa85a33029efd8496c727785536e3b280b0d3880a0c</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-08-31T10:56:41.919440</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -480,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,6 +544,11 @@
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>is_active</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>created_at</t>
         </is>
       </c>
     </row>
@@ -567,12 +609,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>created_by_id</t>
+          <t>created_by</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>lab_id</t>
+          <t>lab_assigned</t>
         </is>
       </c>
     </row>
@@ -587,7 +629,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,7 +645,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>case_id</t>
+          <t>case_number</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -619,6 +661,11 @@
       <c r="E1" s="1" t="inlineStr">
         <is>
           <t>status</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>created_at</t>
         </is>
       </c>
     </row>
@@ -649,17 +696,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>case_id</t>
+          <t>case_number</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>sample_id</t>
+          <t>sample_code</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>actor_id</t>
+          <t>actor</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -685,6 +732,62 @@
       <c r="I1" s="1" t="inlineStr">
         <is>
           <t>hash</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>case_number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>sample_code</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>lab_user</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>result_summary</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>result_file</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>created_at</t>
         </is>
       </c>
     </row>

</xml_diff>